<commit_message>
xlsx is nor possible to upload and display
</commit_message>
<xml_diff>
--- a/frontend/src/components/excel/test.xlsx
+++ b/frontend/src/components/excel/test.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D30320B-B424-4B5B-8422-FB7854F0C50C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A82C1E69-B6D5-4ECF-860C-FA480CC12D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1812" yWindow="648" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,27 +30,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
-  <si>
-    <t>#</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="1">
   <si>
     <t>Bar</t>
-  </si>
-  <si>
-    <t>Line</t>
-  </si>
-  <si>
-    <t>Pie</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Daten</t>
-  </si>
-  <si>
-    <t>Options</t>
   </si>
 </sst>
 </file>
@@ -402,163 +383,174 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="8.109375" customWidth="1"/>
-    <col min="3" max="8" width="6.88671875" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" customWidth="1"/>
+    <col min="3" max="8" width="6.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>1</v>
+      <c r="B1" s="3">
+        <v>12</v>
+      </c>
+      <c r="C1" s="2">
+        <v>24</v>
+      </c>
+      <c r="D1" s="2">
+        <v>48</v>
+      </c>
+      <c r="E1" s="2">
+        <v>96</v>
+      </c>
+      <c r="F1" s="2">
+        <v>192</v>
+      </c>
+      <c r="G1" s="2">
+        <v>256</v>
+      </c>
+      <c r="H1" s="2">
+        <v>512</v>
+      </c>
+      <c r="I1" s="3">
+        <v>1024</v>
+      </c>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3">
+        <v>12</v>
+      </c>
+      <c r="C2" s="2">
+        <v>24</v>
+      </c>
+      <c r="D2" s="2">
+        <v>48</v>
+      </c>
+      <c r="E2" s="2">
+        <v>96</v>
+      </c>
+      <c r="F2" s="2">
+        <v>192</v>
+      </c>
+      <c r="G2" s="2">
+        <v>256</v>
+      </c>
+      <c r="H2" s="2">
+        <v>512</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1024</v>
+      </c>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3">
+        <v>12</v>
       </c>
       <c r="C3" s="2">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" s="2">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="E3" s="2">
-        <v>25</v>
+        <v>96</v>
       </c>
       <c r="F3" s="2">
-        <v>25</v>
+        <v>192</v>
       </c>
       <c r="G3" s="2">
-        <v>25</v>
+        <v>256</v>
       </c>
       <c r="H3" s="2">
-        <v>25</v>
-      </c>
-      <c r="I3" s="3"/>
+        <v>512</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1024</v>
+      </c>
       <c r="J3" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="1">
-        <v>25</v>
-      </c>
-      <c r="D7" s="1">
-        <v>25</v>
-      </c>
-      <c r="E7" s="1">
-        <v>25</v>
-      </c>
-      <c r="F7" s="1">
-        <v>25</v>
-      </c>
-      <c r="G7" s="1">
-        <v>25</v>
-      </c>
-      <c r="H7" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>3</v>
-      </c>
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="1">
-        <v>25</v>
-      </c>
-      <c r="D11" s="1">
-        <v>25</v>
-      </c>
-      <c r="E11" s="1">
-        <v>25</v>
-      </c>
-      <c r="F11" s="1">
-        <v>25</v>
-      </c>
-      <c r="G11" s="1">
-        <v>25</v>
-      </c>
-      <c r="H11" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -572,7 +564,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -584,7 +576,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>